<commit_message>
Fixed coverting excelDate to Javascript date
</commit_message>
<xml_diff>
--- a/api/nigeria-doctors.xlsx
+++ b/api/nigeria-doctors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanAnny\Documents\Final Year Project\Hospital Management System\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD6D439-BF38-4012-83C7-95E6EC1E41D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A33E7D6-D629-46EC-9AC7-DACE947DA7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5352A57C-B09C-4437-925A-ECEE2FF411A7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="336">
   <si>
     <t>Name</t>
   </si>
@@ -1010,7 +1010,40 @@
     <t>LIC000100</t>
   </si>
   <si>
-    <t>2025-06</t>
+    <t>Dr. Lufadeju Dejola</t>
+  </si>
+  <si>
+    <t>lufadeju@dejola.com</t>
+  </si>
+  <si>
+    <t>LIC000101</t>
+  </si>
+  <si>
+    <t>Dr. Ibrahim Michael</t>
+  </si>
+  <si>
+    <t>sim@ibrahin.com</t>
+  </si>
+  <si>
+    <t>LIC000102</t>
+  </si>
+  <si>
+    <t>Dr. Ogunmepo Samuel</t>
+  </si>
+  <si>
+    <t>ogun@dimu.com</t>
+  </si>
+  <si>
+    <t>LIC000103</t>
+  </si>
+  <si>
+    <t>LIC000104</t>
+  </si>
+  <si>
+    <t>goodwin@saka.com</t>
+  </si>
+  <si>
+    <t>Dr. Saka Salami</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1096,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1077,6 +1110,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1412,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDEED1B-8FC0-4B60-9813-98F444B58E43}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="H103" sqref="H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,7 +1465,7 @@
     <col min="6" max="6" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1444,11 +1481,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1468,7 +1505,7 @@
         <v>46022</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1508,7 +1545,7 @@
         <v>45792</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1588,7 +1625,7 @@
         <v>46067</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1608,7 +1645,7 @@
         <v>45847</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
@@ -1628,7 +1665,7 @@
         <v>46130</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -1648,7 +1685,7 @@
         <v>46110</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -1668,7 +1705,7 @@
         <v>45945</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -1688,7 +1725,7 @@
         <v>45992</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>54</v>
       </c>
@@ -1708,7 +1745,7 @@
         <v>46164</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1728,7 +1765,7 @@
         <v>45728</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>61</v>
       </c>
@@ -1748,7 +1785,7 @@
         <v>46031</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>65</v>
       </c>
@@ -1768,7 +1805,7 @@
         <v>45899</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>69</v>
       </c>
@@ -1788,7 +1825,7 @@
         <v>45986</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>72</v>
       </c>
@@ -1808,7 +1845,7 @@
         <v>45554</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>75</v>
       </c>
@@ -1828,7 +1865,7 @@
         <v>45757</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>78</v>
       </c>
@@ -1848,7 +1885,7 @@
         <v>46075</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>81</v>
       </c>
@@ -1868,7 +1905,7 @@
         <v>45823</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>85</v>
       </c>
@@ -1888,7 +1925,7 @@
         <v>46248</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>89</v>
       </c>
@@ -1908,7 +1945,7 @@
         <v>45721</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>92</v>
       </c>
@@ -1928,7 +1965,7 @@
         <v>46011</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>96</v>
       </c>
@@ -1948,7 +1985,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>99</v>
       </c>
@@ -1968,7 +2005,7 @@
         <v>45672</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>102</v>
       </c>
@@ -1988,7 +2025,7 @@
         <v>45922</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>105</v>
       </c>
@@ -2008,7 +2045,7 @@
         <v>46092</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>108</v>
       </c>
@@ -2028,7 +2065,7 @@
         <v>45966</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>111</v>
       </c>
@@ -2048,7 +2085,7 @@
         <v>46040</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>114</v>
       </c>
@@ -2068,7 +2105,7 @@
         <v>45772</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>117</v>
       </c>
@@ -2088,7 +2125,7 @@
         <v>46217</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>120</v>
       </c>
@@ -2108,7 +2145,7 @@
         <v>45780</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>123</v>
       </c>
@@ -2128,7 +2165,7 @@
         <v>45939</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>126</v>
       </c>
@@ -2148,7 +2185,7 @@
         <v>46055</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>129</v>
       </c>
@@ -2168,7 +2205,7 @@
         <v>46021</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>132</v>
       </c>
@@ -2188,7 +2225,7 @@
         <v>45836</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>135</v>
       </c>
@@ -2208,7 +2245,7 @@
         <v>46101</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>138</v>
       </c>
@@ -2228,7 +2265,7 @@
         <v>45972</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>141</v>
       </c>
@@ -2248,7 +2285,7 @@
         <v>45860</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>144</v>
       </c>
@@ -2268,7 +2305,7 @@
         <v>46042</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>147</v>
       </c>
@@ -2288,7 +2325,7 @@
         <v>45874</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>150</v>
       </c>
@@ -2308,7 +2345,7 @@
         <v>46129</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>153</v>
       </c>
@@ -2328,7 +2365,7 @@
         <v>45804</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>156</v>
       </c>
@@ -2348,7 +2385,7 @@
         <v>45993</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>159</v>
       </c>
@@ -2368,7 +2405,7 @@
         <v>46099</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>162</v>
       </c>
@@ -2388,7 +2425,7 @@
         <v>45851</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>165</v>
       </c>
@@ -2408,7 +2445,7 @@
         <v>46081</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>168</v>
       </c>
@@ -2428,7 +2465,7 @@
         <v>45930</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>171</v>
       </c>
@@ -2448,7 +2485,7 @@
         <v>45935</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>174</v>
       </c>
@@ -2468,7 +2505,7 @@
         <v>46034</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>177</v>
       </c>
@@ -2488,7 +2525,7 @@
         <v>45817</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>180</v>
       </c>
@@ -2508,7 +2545,7 @@
         <v>46012</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>183</v>
       </c>
@@ -2528,7 +2565,7 @@
         <v>46210</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>186</v>
       </c>
@@ -2548,7 +2585,7 @@
         <v>45732</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>189</v>
       </c>
@@ -2568,7 +2605,7 @@
         <v>45881</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>192</v>
       </c>
@@ -2588,7 +2625,7 @@
         <v>45751</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>195</v>
       </c>
@@ -2608,7 +2645,7 @@
         <v>46102</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>198</v>
       </c>
@@ -2628,7 +2665,7 @@
         <v>45988</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>201</v>
       </c>
@@ -2648,7 +2685,7 @@
         <v>45945</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>204</v>
       </c>
@@ -2668,7 +2705,7 @@
         <v>46160</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>207</v>
       </c>
@@ -2688,7 +2725,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>210</v>
       </c>
@@ -2708,7 +2745,7 @@
         <v>46022</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>213</v>
       </c>
@@ -2728,7 +2765,7 @@
         <v>45811</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>216</v>
       </c>
@@ -2748,7 +2785,7 @@
         <v>46070</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>219</v>
       </c>
@@ -2768,7 +2805,7 @@
         <v>45941</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>222</v>
       </c>
@@ -2788,7 +2825,7 @@
         <v>45897</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>225</v>
       </c>
@@ -2808,7 +2845,7 @@
         <v>46127</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>228</v>
       </c>
@@ -2828,7 +2865,7 @@
         <v>46015</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>231</v>
       </c>
@@ -2848,7 +2885,7 @@
         <v>45725</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>234</v>
       </c>
@@ -2868,7 +2905,7 @@
         <v>46027</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>237</v>
       </c>
@@ -2888,7 +2925,7 @@
         <v>45867</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>240</v>
       </c>
@@ -2908,7 +2945,7 @@
         <v>46236</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>243</v>
       </c>
@@ -2928,7 +2965,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>246</v>
       </c>
@@ -2948,7 +2985,7 @@
         <v>45788</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>249</v>
       </c>
@@ -2968,7 +3005,7 @@
         <v>46203</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>252</v>
       </c>
@@ -2988,7 +3025,7 @@
         <v>45767</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>255</v>
       </c>
@@ -3008,7 +3045,7 @@
         <v>45896</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>258</v>
       </c>
@@ -3028,7 +3065,7 @@
         <v>46078</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>261</v>
       </c>
@@ -3048,7 +3085,7 @@
         <v>45935</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>264</v>
       </c>
@@ -3068,7 +3105,7 @@
         <v>45973</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>267</v>
       </c>
@@ -3088,7 +3125,7 @@
         <v>46095</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>270</v>
       </c>
@@ -3108,7 +3145,7 @@
         <v>45846</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>273</v>
       </c>
@@ -3128,7 +3165,7 @@
         <v>45674</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>276</v>
       </c>
@@ -3148,7 +3185,7 @@
         <v>46117</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>279</v>
       </c>
@@ -3168,7 +3205,7 @@
         <v>45819</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>282</v>
       </c>
@@ -3188,7 +3225,7 @@
         <v>45962</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>285</v>
       </c>
@@ -3208,7 +3245,7 @@
         <v>46207</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>288</v>
       </c>
@@ -3228,7 +3265,7 @@
         <v>45731</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>291</v>
       </c>
@@ -3248,7 +3285,7 @@
         <v>46008</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>294</v>
       </c>
@@ -3268,7 +3305,7 @@
         <v>46046</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>297</v>
       </c>
@@ -3288,7 +3325,7 @@
         <v>45928</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>300</v>
       </c>
@@ -3308,7 +3345,7 @@
         <v>45800</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>303</v>
       </c>
@@ -3328,7 +3365,7 @@
         <v>45887</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>306</v>
       </c>
@@ -3348,7 +3385,7 @@
         <v>46224</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>309</v>
       </c>
@@ -3368,7 +3405,7 @@
         <v>45937</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>312</v>
       </c>
@@ -3388,7 +3425,7 @@
         <v>45763</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>315</v>
       </c>
@@ -3408,7 +3445,7 @@
         <v>46065</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>318</v>
       </c>
@@ -3428,7 +3465,7 @@
         <v>45676</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>321</v>
       </c>
@@ -3444,16 +3481,96 @@
       <c r="E101" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F101" s="4">
+        <v>44945</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
         <v>324</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F102" s="4">
+        <v>46041</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F103" s="4">
+        <v>45962</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F104" s="4">
+        <v>45676</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F105" s="4">
+        <v>45676</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="mailto:john.doe@example.com" xr:uid="{A9F47AA3-E2FC-4B49-9578-DF63F7922727}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{A9F47AA3-E2FC-4B49-9578-DF63F7922727}"/>
     <hyperlink ref="D3" r:id="rId2" display="mailto:jane.smith@example.com" xr:uid="{C54C5332-913B-4739-BFEC-A27D926DDDCD}"/>
     <hyperlink ref="D4" r:id="rId3" display="mailto:ahmed.bello@example.com" xr:uid="{612DA7A9-B496-4AB3-8387-9449DE036C1C}"/>
-    <hyperlink ref="D5" r:id="rId4" display="mailto:mary.johnson@example.com" xr:uid="{3F9AD872-D5B8-43C9-95E6-2F41587D9579}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{3F9AD872-D5B8-43C9-95E6-2F41587D9579}"/>
     <hyperlink ref="D6" r:id="rId5" display="mailto:samuel.okeke@example.com" xr:uid="{01A3AEAC-EFFF-46FD-8394-085BD50D90D3}"/>
     <hyperlink ref="D7" r:id="rId6" display="mailto:chika.nwosu@example.com" xr:uid="{90C4713F-C6BC-4104-BB33-C1A73BF45C68}"/>
     <hyperlink ref="D8" r:id="rId7" display="mailto:peter.adebayo@example.com" xr:uid="{E086C44C-8B35-4300-9775-1BD55B997889}"/>
@@ -3550,7 +3667,12 @@
     <hyperlink ref="D99" r:id="rId98" display="mailto:fola.alabi@example.com" xr:uid="{5BD76884-B114-4E79-899D-81C722DAD0AD}"/>
     <hyperlink ref="D100" r:id="rId99" display="mailto:chuka.ibe@example.com" xr:uid="{E4EE7EC8-F0FC-4269-B7B8-3F6F3E75A1A5}"/>
     <hyperlink ref="D101" r:id="rId100" display="mailto:nneka.opara@example.com" xr:uid="{EEFDFFA6-57AA-47DE-81D6-64D68360240F}"/>
+    <hyperlink ref="D102" r:id="rId101" xr:uid="{4A067958-46E5-4DC8-A52D-9CF4B24B6139}"/>
+    <hyperlink ref="D103" r:id="rId102" xr:uid="{2CE30148-F583-44DE-97DB-B113326F7C83}"/>
+    <hyperlink ref="D104" r:id="rId103" xr:uid="{F53BD952-723F-4474-93CC-6960116B50E2}"/>
+    <hyperlink ref="D105" r:id="rId104" xr:uid="{EB1641C1-AA0D-4DC8-B90A-BEAD65608E53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId105"/>
 </worksheet>
 </file>
</xml_diff>